<commit_message>
collateral tambahan motor, mobil, corporate & import partner
</commit_message>
<xml_diff>
--- a/public/data_file/debitur.xlsx
+++ b/public/data_file/debitur.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A17FA4D3-4A66-4EEC-B78B-E8739D13D5FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A209B1-3E2E-408E-B14A-7E98D6A796F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DD82610D-797C-4253-ACE6-E74E470448B8}"/>
   </bookViews>
@@ -33,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
-  <si>
-    <t>M. ALVIN</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
   <si>
     <t>08.199.566.3-123.323</t>
   </si>
@@ -74,9 +71,6 @@
     <t>YA</t>
   </si>
   <si>
-    <t>BAGUS WICAKSANA</t>
-  </si>
-  <si>
     <t>Jl. Keranji No.58</t>
   </si>
   <si>
@@ -93,6 +87,81 @@
   </si>
   <si>
     <t>TRUCK</t>
+  </si>
+  <si>
+    <t>NAMA_DEBITUR</t>
+  </si>
+  <si>
+    <t>TANGGAL_LAHIR</t>
+  </si>
+  <si>
+    <t>NO_KTP</t>
+  </si>
+  <si>
+    <t>NO_NPWP</t>
+  </si>
+  <si>
+    <t>ALAMAT_CUSTOMER</t>
+  </si>
+  <si>
+    <t>PROVINSI</t>
+  </si>
+  <si>
+    <t>KABUPATEN_KOTA</t>
+  </si>
+  <si>
+    <t>KECAMATAN</t>
+  </si>
+  <si>
+    <t>KELURAHAN</t>
+  </si>
+  <si>
+    <t>KODE_POS</t>
+  </si>
+  <si>
+    <t>NAMA_PERUSAHAAN</t>
+  </si>
+  <si>
+    <t>BIDANG_USAHA</t>
+  </si>
+  <si>
+    <t>SUB_BIDANG_USAHA</t>
+  </si>
+  <si>
+    <t>LAMA_USAHA</t>
+  </si>
+  <si>
+    <t>JABATAN</t>
+  </si>
+  <si>
+    <t>TANGGUNGAN</t>
+  </si>
+  <si>
+    <t>INCOME_BULAN</t>
+  </si>
+  <si>
+    <t>SUPOUSE_INCOME_BULAN</t>
+  </si>
+  <si>
+    <t>REKENING_KORAN_3_BULAN_TERAKHIR_BULAN_1</t>
+  </si>
+  <si>
+    <t>REKENING_KORAN_3_BULAN_TERAKHIR_BULAN_2</t>
+  </si>
+  <si>
+    <t>REKENING_KORAN_3_BULAN_TERAKHIR_BULAN_3</t>
+  </si>
+  <si>
+    <t>APAKAH_ADA_DP</t>
+  </si>
+  <si>
+    <t>DOWN_PAYMENT_CUSTOMER</t>
+  </si>
+  <si>
+    <t>M. REZA</t>
+  </si>
+  <si>
+    <t>DIMAS HAIDAR</t>
   </si>
 </sst>
 </file>
@@ -100,8 +169,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="d/mm/yyyy;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -134,9 +203,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,160 +520,253 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D1298A0-44C4-4729-B91A-A465C0FD90E6}">
-  <dimension ref="C1:Y2"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" customWidth="1"/>
+    <col min="3" max="4" width="19.21875" customWidth="1"/>
+    <col min="5" max="5" width="22" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="8" max="8" width="20.44140625" customWidth="1"/>
+    <col min="9" max="9" width="17.44140625" customWidth="1"/>
+    <col min="10" max="10" width="21.77734375" customWidth="1"/>
+    <col min="11" max="11" width="21.5546875" customWidth="1"/>
+    <col min="12" max="12" width="21.77734375" customWidth="1"/>
+    <col min="13" max="13" width="20.21875" customWidth="1"/>
+    <col min="14" max="14" width="18.6640625" customWidth="1"/>
+    <col min="15" max="15" width="17.77734375" customWidth="1"/>
+    <col min="16" max="16" width="16.5546875" customWidth="1"/>
+    <col min="17" max="17" width="18.44140625" customWidth="1"/>
+    <col min="18" max="18" width="27.77734375" customWidth="1"/>
+    <col min="19" max="19" width="43.88671875" customWidth="1"/>
+    <col min="20" max="20" width="44.44140625" customWidth="1"/>
+    <col min="21" max="21" width="46.5546875" customWidth="1"/>
+    <col min="22" max="22" width="19.77734375" customWidth="1"/>
+    <col min="23" max="23" width="27.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
       <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>34</v>
+      </c>
+      <c r="R1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S1" t="s">
+        <v>36</v>
+      </c>
+      <c r="T1" t="s">
+        <v>37</v>
+      </c>
+      <c r="U1" t="s">
+        <v>38</v>
+      </c>
+      <c r="V1" t="s">
+        <v>39</v>
+      </c>
+      <c r="W1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="2">
+        <v>35015</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2133123213122130</v>
+      </c>
+      <c r="D2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3">
-        <v>35015</v>
-      </c>
-      <c r="E1" s="2">
-        <v>2133123213122130</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="E2" t="s">
         <v>1</v>
       </c>
-      <c r="G1" t="s">
+      <c r="F2" t="s">
         <v>2</v>
       </c>
-      <c r="H1" t="s">
+      <c r="G2" t="s">
         <v>3</v>
       </c>
-      <c r="I1" t="s">
+      <c r="H2" t="s">
         <v>4</v>
       </c>
-      <c r="J1" t="s">
+      <c r="I2" t="s">
         <v>5</v>
       </c>
-      <c r="K1" t="s">
+      <c r="J2" s="1">
+        <v>16542</v>
+      </c>
+      <c r="K2" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="2">
-        <v>16542</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="L2" t="s">
         <v>7</v>
       </c>
-      <c r="N1" t="s">
+      <c r="M2" t="s">
         <v>8</v>
       </c>
-      <c r="O1" t="s">
+      <c r="N2" t="s">
         <v>9</v>
       </c>
-      <c r="P1" t="s">
+      <c r="O2" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="P2" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>10000000</v>
+      </c>
+      <c r="R2" s="1">
+        <v>5000000</v>
+      </c>
+      <c r="S2" s="1">
+        <v>20000000</v>
+      </c>
+      <c r="T2" s="1">
+        <v>30000000</v>
+      </c>
+      <c r="U2" s="1">
+        <v>40000000</v>
+      </c>
+      <c r="V2" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="2">
+      <c r="W2" s="1">
+        <v>5000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="3">
+        <v>35016</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2565476865776570</v>
+      </c>
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
         <v>2</v>
       </c>
-      <c r="S1" s="2">
-        <v>10000000</v>
-      </c>
-      <c r="T1" s="2">
+      <c r="G3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="1">
+        <v>16453</v>
+      </c>
+      <c r="K3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N3" t="s">
+        <v>9</v>
+      </c>
+      <c r="O3" t="s">
+        <v>10</v>
+      </c>
+      <c r="P3" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>15000000</v>
+      </c>
+      <c r="R3" s="1">
         <v>5000000</v>
       </c>
-      <c r="U1" s="2">
+      <c r="S3" s="1">
         <v>20000000</v>
       </c>
-      <c r="V1" s="2">
+      <c r="T3" s="1">
         <v>30000000</v>
       </c>
-      <c r="W1" s="2">
+      <c r="U3" s="1">
         <v>40000000</v>
       </c>
-      <c r="X1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y1" s="2">
-        <v>5000000</v>
-      </c>
-    </row>
-    <row r="2" spans="3:25" x14ac:dyDescent="0.3">
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="1">
-        <v>35016</v>
-      </c>
-      <c r="E2" s="2">
-        <v>2565476865776570</v>
-      </c>
-      <c r="F2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L2" s="2">
-        <v>16453</v>
-      </c>
-      <c r="M2" t="s">
-        <v>17</v>
-      </c>
-      <c r="N2" t="s">
-        <v>18</v>
-      </c>
-      <c r="O2" t="s">
-        <v>19</v>
-      </c>
-      <c r="P2" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q2" t="s">
+      <c r="V3" t="s">
         <v>11</v>
       </c>
-      <c r="R2" s="2">
-        <v>3</v>
-      </c>
-      <c r="S2" s="2">
-        <v>15000000</v>
-      </c>
-      <c r="T2" s="2">
-        <v>5000000</v>
-      </c>
-      <c r="U2" s="2">
-        <v>20000000</v>
-      </c>
-      <c r="V2" s="2">
-        <v>30000000</v>
-      </c>
-      <c r="W2" s="2">
-        <v>40000000</v>
-      </c>
-      <c r="X2" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y2" s="2">
+      <c r="W3" s="1">
         <v>5000000</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>